<commit_message>
Completed Excel DSUM Function Single Criteria Continued
</commit_message>
<xml_diff>
--- a/15 - Excel List Functions/Excel102Exercises.xlsx
+++ b/15 - Excel List Functions/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/15 - Excel List Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4860AFA2-0706-44AA-9297-B51F74C5B164}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{255C8126-BF8C-4CD6-9DCA-7907C4823641}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5043" uniqueCount="1433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="1433">
   <si>
     <t>Town</t>
   </si>
@@ -4558,7 +4558,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -4869,6 +4869,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4879,7 +4888,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -5058,6 +5067,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -8750,10 +8760,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8764,9 +8774,10 @@
     <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" customWidth="1"/>
     <col min="6" max="6" width="13.7265625" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="72" t="s">
         <v>119</v>
       </c>
@@ -8786,7 +8797,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>116</v>
       </c>
@@ -8806,11 +8817,14 @@
         <f t="shared" ref="F2:F33" si="0">SUM(C2:E2)</f>
         <v>2150</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="82" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="I2" s="82" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>116</v>
       </c>
@@ -8833,8 +8847,12 @@
       <c r="H3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <f>DSUM(A1:F59,F1,H2:H3)</f>
+        <v>71160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>116</v>
       </c>
@@ -8855,7 +8873,7 @@
         <v>9205</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>116</v>
       </c>
@@ -8876,7 +8894,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>116</v>
       </c>
@@ -8897,7 +8915,7 @@
         <v>5875</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>116</v>
       </c>
@@ -8918,7 +8936,7 @@
         <v>4550</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>116</v>
       </c>
@@ -8939,7 +8957,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>116</v>
       </c>
@@ -8960,7 +8978,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>116</v>
       </c>
@@ -8981,7 +8999,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>116</v>
       </c>
@@ -9002,7 +9020,7 @@
         <v>18750</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>116</v>
       </c>
@@ -9023,7 +9041,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>116</v>
       </c>
@@ -9044,7 +9062,7 @@
         <v>36500</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
         <v>116</v>
       </c>
@@ -9065,7 +9083,7 @@
         <v>37250</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
         <v>116</v>
       </c>
@@ -9086,7 +9104,7 @@
         <v>75390</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Completed Excel DSUM Function with OR Criteria
</commit_message>
<xml_diff>
--- a/15 - Excel List Functions/Excel102Exercises.xlsx
+++ b/15 - Excel List Functions/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/15 - Excel List Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{255C8126-BF8C-4CD6-9DCA-7907C4823641}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ECC9E96-A78D-416A-9371-7E6909AE6150}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="1433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5045" uniqueCount="1433">
   <si>
     <t>Town</t>
   </si>
@@ -5055,6 +5055,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5067,7 +5068,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -7423,14 +7423,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
     </row>
     <row r="2" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.3">
@@ -8763,7 +8763,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8817,10 +8817,10 @@
         <f t="shared" ref="F2:F33" si="0">SUM(C2:E2)</f>
         <v>2150</v>
       </c>
-      <c r="H2" s="82" t="s">
+      <c r="H2" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="82" t="s">
+      <c r="I2" s="78" t="s">
         <v>1394</v>
       </c>
     </row>
@@ -8848,8 +8848,8 @@
         <v>130</v>
       </c>
       <c r="I3">
-        <f>DSUM(A1:F59,F1,H2:H3)</f>
-        <v>71160</v>
+        <f>DSUM(A1:F59,F1,H2:H4)</f>
+        <v>88375</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -8871,6 +8871,9 @@
       <c r="F4" s="39">
         <f t="shared" si="0"/>
         <v>9205</v>
+      </c>
+      <c r="H4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
@@ -10062,28 +10065,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>743</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
     </row>
     <row r="3" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="45"/>

</xml_diff>

<commit_message>
Completed Excel DSUM Function with AND Criteria
</commit_message>
<xml_diff>
--- a/15 - Excel List Functions/Excel102Exercises.xlsx
+++ b/15 - Excel List Functions/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/15 - Excel List Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ECC9E96-A78D-416A-9371-7E6909AE6150}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F653D95D-AF95-45ED-B306-81B337C86B12}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5045" uniqueCount="1433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5048" uniqueCount="1433">
   <si>
     <t>Town</t>
   </si>
@@ -8760,10 +8760,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8774,10 +8774,10 @@
     <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" customWidth="1"/>
     <col min="6" max="6" width="13.7265625" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="72" t="s">
         <v>119</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>116</v>
       </c>
@@ -8818,13 +8818,16 @@
         <v>2150</v>
       </c>
       <c r="H2" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="J2" s="78" t="s">
         <v>1394</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>116</v>
       </c>
@@ -8845,14 +8848,17 @@
         <v>2600</v>
       </c>
       <c r="H3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" t="s">
         <v>130</v>
       </c>
-      <c r="I3">
-        <f>DSUM(A1:F59,F1,H2:H4)</f>
-        <v>88375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <f>DSUM(A1:F59,F1,H2:I4)</f>
+        <v>21865</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>116</v>
       </c>
@@ -8873,10 +8879,13 @@
         <v>9205</v>
       </c>
       <c r="H4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>116</v>
       </c>
@@ -8897,7 +8906,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>116</v>
       </c>
@@ -8918,7 +8927,7 @@
         <v>5875</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>116</v>
       </c>
@@ -8939,7 +8948,7 @@
         <v>4550</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>116</v>
       </c>
@@ -8960,7 +8969,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>116</v>
       </c>
@@ -8981,7 +8990,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>116</v>
       </c>
@@ -9002,7 +9011,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>116</v>
       </c>
@@ -9023,7 +9032,7 @@
         <v>18750</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>116</v>
       </c>
@@ -9044,7 +9053,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>116</v>
       </c>
@@ -9065,7 +9074,7 @@
         <v>36500</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
         <v>116</v>
       </c>
@@ -9086,7 +9095,7 @@
         <v>37250</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
         <v>116</v>
       </c>
@@ -9107,7 +9116,7 @@
         <v>75390</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Completed Excel Function: DAVERAGE()
</commit_message>
<xml_diff>
--- a/15 - Excel List Functions/Excel102Exercises.xlsx
+++ b/15 - Excel List Functions/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/15 - Excel List Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F653D95D-AF95-45ED-B306-81B337C86B12}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63D331D9-81B9-4D1A-84A8-ABD0B65D051A}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5048" uniqueCount="1433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5049" uniqueCount="1435">
   <si>
     <t>Town</t>
   </si>
@@ -4353,6 +4353,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>SUM Total Sales</t>
+  </si>
+  <si>
+    <t>AVG Total Sales</t>
   </si>
 </sst>
 </file>
@@ -4888,7 +4894,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -5068,6 +5074,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -8760,10 +8767,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8774,10 +8781,11 @@
     <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" customWidth="1"/>
     <col min="6" max="6" width="13.7265625" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="72" t="s">
         <v>119</v>
       </c>
@@ -8797,7 +8805,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>116</v>
       </c>
@@ -8824,10 +8832,13 @@
         <v>120</v>
       </c>
       <c r="J2" s="78" t="s">
-        <v>1394</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+        <v>1433</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>116</v>
       </c>
@@ -8853,12 +8864,16 @@
       <c r="I3" t="s">
         <v>130</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="83">
         <f>DSUM(A1:F59,F1,H2:I4)</f>
         <v>21865</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="K3" s="83">
+        <f>DAVERAGE(A1:F59,F1,H2:I4)</f>
+        <v>10932.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>116</v>
       </c>
@@ -8885,7 +8900,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>116</v>
       </c>
@@ -8906,7 +8921,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>116</v>
       </c>
@@ -8927,7 +8942,7 @@
         <v>5875</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>116</v>
       </c>
@@ -8948,7 +8963,7 @@
         <v>4550</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>116</v>
       </c>
@@ -8969,7 +8984,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>116</v>
       </c>
@@ -8990,7 +9005,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>116</v>
       </c>
@@ -9011,7 +9026,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>116</v>
       </c>
@@ -9032,7 +9047,7 @@
         <v>18750</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>116</v>
       </c>
@@ -9053,7 +9068,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>116</v>
       </c>
@@ -9074,7 +9089,7 @@
         <v>36500</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
         <v>116</v>
       </c>
@@ -9095,7 +9110,7 @@
         <v>37250</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
         <v>116</v>
       </c>
@@ -9116,7 +9131,7 @@
         <v>75390</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Completed Excel Function: DCOUNT()
</commit_message>
<xml_diff>
--- a/15 - Excel List Functions/Excel102Exercises.xlsx
+++ b/15 - Excel List Functions/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/15 - Excel List Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63D331D9-81B9-4D1A-84A8-ABD0B65D051A}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E263DF39-4D55-4457-B9DC-852BA436C7F7}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5049" uniqueCount="1435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5053" uniqueCount="1436">
   <si>
     <t>Town</t>
   </si>
@@ -4359,6 +4359,9 @@
   </si>
   <si>
     <t>AVG Total Sales</t>
+  </si>
+  <si>
+    <t>COUNT</t>
   </si>
 </sst>
 </file>
@@ -4894,7 +4897,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -5062,6 +5065,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5074,7 +5078,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -7430,14 +7434,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
     </row>
     <row r="2" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.3">
@@ -8769,8 +8773,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8864,11 +8868,11 @@
       <c r="I3" t="s">
         <v>130</v>
       </c>
-      <c r="J3" s="83">
+      <c r="J3" s="79">
         <f>DSUM(A1:F59,F1,H2:I4)</f>
         <v>21865</v>
       </c>
-      <c r="K3" s="83">
+      <c r="K3" s="79">
         <f>DAVERAGE(A1:F59,F1,H2:I4)</f>
         <v>10932.5</v>
       </c>
@@ -8962,6 +8966,15 @@
         <f t="shared" si="0"/>
         <v>4550</v>
       </c>
+      <c r="H7" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="78" t="s">
+        <v>1435</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
@@ -8983,6 +8996,14 @@
         <f t="shared" si="0"/>
         <v>10500</v>
       </c>
+      <c r="I8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="84">
+        <f>DCOUNTA(A1:F59,B1,H7:I8)</f>
+        <v>4</v>
+      </c>
+      <c r="K8" s="79"/>
     </row>
     <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
@@ -10089,28 +10110,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="83" t="s">
         <v>743</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
     </row>
     <row r="3" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="45"/>

</xml_diff>

<commit_message>
Completed Excel Function: SUBTOTAL()
</commit_message>
<xml_diff>
--- a/15 - Excel List Functions/Excel102Exercises.xlsx
+++ b/15 - Excel List Functions/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/15 - Excel List Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E263DF39-4D55-4457-B9DC-852BA436C7F7}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{130A0F1D-8EC9-40A6-AE08-F197F3DAF875}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5053" uniqueCount="1436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5055" uniqueCount="1438">
   <si>
     <t>Town</t>
   </si>
@@ -4362,6 +4362,12 @@
   </si>
   <si>
     <t>COUNT</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
   </si>
 </sst>
 </file>
@@ -5066,6 +5072,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5078,7 +5085,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -7434,14 +7440,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
     </row>
     <row r="2" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.3">
@@ -8774,7 +8780,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8785,6 +8791,7 @@
     <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" customWidth="1"/>
     <col min="6" max="6" width="13.7265625" customWidth="1"/>
+    <col min="8" max="9" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8999,7 +9006,7 @@
       <c r="I8" t="s">
         <v>126</v>
       </c>
-      <c r="J8" s="84">
+      <c r="J8" s="80">
         <f>DCOUNTA(A1:F59,B1,H7:I8)</f>
         <v>4</v>
       </c>
@@ -9067,6 +9074,12 @@
         <f t="shared" si="0"/>
         <v>18750</v>
       </c>
+      <c r="H11" s="78" t="s">
+        <v>1436</v>
+      </c>
+      <c r="I11" s="78" t="s">
+        <v>1437</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
@@ -9087,6 +9100,14 @@
       <c r="F12" s="39">
         <f t="shared" si="0"/>
         <v>24000</v>
+      </c>
+      <c r="H12" s="79">
+        <f>SUM(F1:F59)</f>
+        <v>1428320</v>
+      </c>
+      <c r="I12" s="79">
+        <f>SUBTOTAL(9,F2:F59)</f>
+        <v>1428320</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -10110,28 +10131,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="84" t="s">
         <v>743</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="45"/>

</xml_diff>